<commit_message>
Writes Data with Headers Properly
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -15,7 +15,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>FIRST</t>
+  </si>
+  <si>
+    <t>SECOND</t>
+  </si>
+  <si>
+    <t>THIRD</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,7 +368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -358,46 +377,68 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="n">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="n">
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="n">
         <v>11</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B5" t="n">
         <v>12</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C5" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="n">
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
         <v>21</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B6" t="n">
         <v>22</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C6" t="n">
         <v>23</v>
       </c>
     </row>

</xml_diff>